<commit_message>
Add lab blue beam charts and text
</commit_message>
<xml_diff>
--- a/tables/porownanie_modow_test_blue.xlsx
+++ b/tables/porownanie_modow_test_blue.xlsx
@@ -1,21 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23530"/>
-  <workbookPr defaultThemeVersion="166925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\DR\doktorat_v01\Latex\phd_kali\tables\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Dane\Doktorat\phd_kalitowski\phd_kali\tables\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{DBCE438F-3682-4685-A4E6-EC4C5A393DBD}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{BD9E99A6-C956-4778-8F31-B58CCBEAD632}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15996"/>
   </bookViews>
   <sheets>
     <sheet name="Arkusz1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -34,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="21">
   <si>
     <t>Mod 1</t>
   </si>
@@ -102,9 +101,10 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <numFmts count="2">
     <numFmt numFmtId="164" formatCode="0.0000"/>
+    <numFmt numFmtId="165" formatCode="0.000"/>
   </numFmts>
   <fonts count="4" x14ac:knownFonts="1">
     <font>
@@ -161,7 +161,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -178,13 +178,25 @@
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -501,22 +513,23 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{06E7A704-6F95-45C9-9D3C-3A8C2D84B413}">
-  <dimension ref="A1:M11"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:M28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J15" sqref="J15"/>
+      <selection activeCell="H25" sqref="H25:H28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="19.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="13.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="6.140625" customWidth="1"/>
-    <col min="4" max="4" width="7.5703125" customWidth="1"/>
+    <col min="1" max="1" width="19.44140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="6.109375" customWidth="1"/>
+    <col min="4" max="4" width="7.5546875" customWidth="1"/>
+    <col min="7" max="7" width="9.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.3">
       <c r="D1" s="1" t="s">
         <v>0</v>
       </c>
@@ -548,7 +561,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>10</v>
       </c>
@@ -589,7 +602,7 @@
         <v>451.89</v>
       </c>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
         <v>13</v>
       </c>
@@ -630,8 +643,8 @@
         <v>7.6495228226633322E-2</v>
       </c>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A4" s="6" t="s">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A4" s="8" t="s">
         <v>16</v>
       </c>
       <c r="B4" t="s">
@@ -671,46 +684,46 @@
         <v>17</v>
       </c>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A5" s="6"/>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A5" s="8"/>
       <c r="B5" t="s">
         <v>18</v>
       </c>
       <c r="C5" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="D5" s="7">
-        <f>D4/D2</f>
+      <c r="D5" s="6">
+        <f t="shared" ref="D5:I5" si="0">D4/D2</f>
         <v>0.99650986342943859</v>
       </c>
-      <c r="E5" s="7">
-        <f>E4/E2</f>
+      <c r="E5" s="6">
+        <f t="shared" si="0"/>
         <v>1.0005097396686693</v>
       </c>
-      <c r="F5" s="7">
-        <f>F4/F2</f>
+      <c r="F5" s="6">
+        <f t="shared" si="0"/>
         <v>0.9888874680306905</v>
       </c>
-      <c r="G5" s="7">
-        <f>G4/G2</f>
+      <c r="G5" s="6">
+        <f t="shared" si="0"/>
         <v>0.9792066935233964</v>
       </c>
-      <c r="H5" s="7">
-        <f>H4/H2</f>
+      <c r="H5" s="6">
+        <f t="shared" si="0"/>
         <v>0.98752869547859068</v>
       </c>
-      <c r="I5" s="7">
-        <f>I4/I2</f>
+      <c r="I5" s="6">
+        <f t="shared" si="0"/>
         <v>0.96725405201658488</v>
       </c>
-      <c r="J5" s="7" t="s">
-        <v>17</v>
-      </c>
-      <c r="K5" s="7">
+      <c r="J5" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="K5" s="6">
         <f>K4/K2</f>
         <v>0.92347960426631814</v>
       </c>
-      <c r="L5" s="7">
+      <c r="L5" s="6">
         <f>L4/L2</f>
         <v>0.9375920237921116</v>
       </c>
@@ -718,8 +731,8 @@
         <v>17</v>
       </c>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A6" s="6"/>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A6" s="8"/>
       <c r="B6" t="s">
         <v>14</v>
       </c>
@@ -757,55 +770,55 @@
         <v>17</v>
       </c>
     </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A7" s="6"/>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A7" s="8"/>
       <c r="B7" t="s">
         <v>18</v>
       </c>
       <c r="C7" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="D7" s="7">
-        <f>D6/D3</f>
+      <c r="D7" s="6">
+        <f t="shared" ref="D7:I7" si="1">D6/D3</f>
         <v>0.9612874980203171</v>
       </c>
-      <c r="E7" s="7">
-        <f>E6/E3</f>
+      <c r="E7" s="6">
+        <f t="shared" si="1"/>
         <v>1.2298344898607112</v>
       </c>
-      <c r="F7" s="7">
-        <f>F6/F3</f>
+      <c r="F7" s="6">
+        <f t="shared" si="1"/>
         <v>0.95701237971324415</v>
       </c>
-      <c r="G7" s="7">
-        <f>G6/G3</f>
+      <c r="G7" s="6">
+        <f t="shared" si="1"/>
         <v>0.79477803492854915</v>
       </c>
-      <c r="H7" s="7">
-        <f>H6/H3</f>
+      <c r="H7" s="6">
+        <f t="shared" si="1"/>
         <v>0.90131873614999336</v>
       </c>
-      <c r="I7" s="7">
-        <f>I6/I3</f>
+      <c r="I7" s="6">
+        <f t="shared" si="1"/>
         <v>1.0821878993299516</v>
       </c>
-      <c r="J7" s="7" t="s">
-        <v>17</v>
-      </c>
-      <c r="K7" s="7">
+      <c r="J7" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="K7" s="6">
         <f>K6/K3</f>
         <v>0.82000105549845459</v>
       </c>
-      <c r="L7" s="7">
+      <c r="L7" s="6">
         <f>L6/L3</f>
         <v>0.90139078502666203</v>
       </c>
-      <c r="M7" s="7" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A8" s="8" t="s">
+      <c r="M7" s="6" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A8" s="9" t="s">
         <v>20</v>
       </c>
       <c r="B8" t="s">
@@ -814,32 +827,268 @@
       <c r="C8" s="3" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A9" s="8"/>
+      <c r="D8" s="3">
+        <v>20.466999999999999</v>
+      </c>
+      <c r="E8" s="3">
+        <v>22.236000000000001</v>
+      </c>
+      <c r="F8" s="3">
+        <v>76.739000000000004</v>
+      </c>
+      <c r="G8" s="3">
+        <v>163.584</v>
+      </c>
+      <c r="H8" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="I8" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="J8" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="K8" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="L8" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="M8" s="6" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A9" s="9"/>
       <c r="B9" t="s">
         <v>18</v>
       </c>
       <c r="C9" s="3" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A10" s="8"/>
+      <c r="D9" s="6">
+        <f>D8/D2</f>
+        <v>1.0352554375316134</v>
+      </c>
+      <c r="E9" s="6">
+        <f t="shared" ref="E9:G9" si="2">E8/E2</f>
+        <v>0.40480611687602402</v>
+      </c>
+      <c r="F9" s="6">
+        <f t="shared" si="2"/>
+        <v>0.9813171355498721</v>
+      </c>
+      <c r="G9" s="6">
+        <f t="shared" si="2"/>
+        <v>1.0138456770994733</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A10" s="9"/>
       <c r="B10" t="s">
         <v>14</v>
       </c>
       <c r="C10" s="3" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A11" s="8"/>
+      <c r="D10" s="10">
+        <v>0.11749556524425828</v>
+      </c>
+      <c r="E10" s="10">
+        <v>0.44045129003328898</v>
+      </c>
+      <c r="F10" s="10">
+        <v>0.15079644737231007</v>
+      </c>
+      <c r="G10" s="10">
+        <v>0.18535396656179778</v>
+      </c>
+      <c r="H10" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="I10" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="J10" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="K10" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="L10" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="M10" s="6" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A11" s="9"/>
       <c r="B11" t="s">
         <v>18</v>
       </c>
       <c r="C11" s="3" t="s">
         <v>19</v>
+      </c>
+      <c r="D11" s="6">
+        <f>D10/D3</f>
+        <v>3.8813408227538133</v>
+      </c>
+      <c r="E11" s="6">
+        <f t="shared" ref="E11:G11" si="3">E10/E3</f>
+        <v>23.348370154594058</v>
+      </c>
+      <c r="F11" s="6">
+        <f t="shared" si="3"/>
+        <v>7.595477208004076</v>
+      </c>
+      <c r="G11" s="6">
+        <f t="shared" si="3"/>
+        <v>6.1381358879249017</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="D13">
+        <f>D14*2*PI()</f>
+        <v>0.11749556524425828</v>
+      </c>
+      <c r="E13">
+        <f t="shared" ref="E13:G13" si="4">E14*2*PI()</f>
+        <v>0.44045129003328898</v>
+      </c>
+      <c r="F13">
+        <f t="shared" si="4"/>
+        <v>0.15079644737231007</v>
+      </c>
+      <c r="G13">
+        <f t="shared" si="4"/>
+        <v>0.18535396656179778</v>
+      </c>
+    </row>
+    <row r="14" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="D14">
+        <v>1.8700000000000001E-2</v>
+      </c>
+      <c r="E14">
+        <v>7.0099999999999996E-2</v>
+      </c>
+      <c r="F14">
+        <v>2.4E-2</v>
+      </c>
+      <c r="G14">
+        <v>2.9499999999999998E-2</v>
+      </c>
+    </row>
+    <row r="19" spans="5:8" x14ac:dyDescent="0.3">
+      <c r="E19">
+        <v>20.466999999999999</v>
+      </c>
+      <c r="F19">
+        <v>22.236000000000001</v>
+      </c>
+      <c r="G19">
+        <v>76.739000000000004</v>
+      </c>
+      <c r="H19">
+        <v>163.584</v>
+      </c>
+    </row>
+    <row r="20" spans="5:8" x14ac:dyDescent="0.3">
+      <c r="E20">
+        <v>1.0352554375316134</v>
+      </c>
+      <c r="F20">
+        <v>0.40480611687602402</v>
+      </c>
+      <c r="G20">
+        <v>0.9813171355498721</v>
+      </c>
+      <c r="H20">
+        <v>1.0138456770994733</v>
+      </c>
+    </row>
+    <row r="21" spans="5:8" x14ac:dyDescent="0.3">
+      <c r="E21">
+        <v>0.11749556524425828</v>
+      </c>
+      <c r="F21">
+        <v>0.44045129003328898</v>
+      </c>
+      <c r="G21">
+        <v>0.15079644737231007</v>
+      </c>
+      <c r="H21">
+        <v>0.18535396656179778</v>
+      </c>
+    </row>
+    <row r="22" spans="5:8" x14ac:dyDescent="0.3">
+      <c r="E22">
+        <v>3.8813408227538133</v>
+      </c>
+      <c r="F22">
+        <v>23.348370154594058</v>
+      </c>
+      <c r="G22">
+        <v>7.595477208004076</v>
+      </c>
+      <c r="H22">
+        <v>6.1381358879249017</v>
+      </c>
+    </row>
+    <row r="25" spans="5:8" x14ac:dyDescent="0.3">
+      <c r="E25" s="7">
+        <v>20.466999999999999</v>
+      </c>
+      <c r="F25" s="11">
+        <v>1.0352554375316134</v>
+      </c>
+      <c r="G25" s="12">
+        <v>0.11749556524425828</v>
+      </c>
+      <c r="H25" s="11">
+        <v>3.8813408227538133</v>
+      </c>
+    </row>
+    <row r="26" spans="5:8" x14ac:dyDescent="0.3">
+      <c r="E26" s="7">
+        <v>22.236000000000001</v>
+      </c>
+      <c r="F26" s="11">
+        <v>0.40480611687602402</v>
+      </c>
+      <c r="G26" s="12">
+        <v>0.44045129003328898</v>
+      </c>
+      <c r="H26" s="11">
+        <v>23.348370154594058</v>
+      </c>
+    </row>
+    <row r="27" spans="5:8" x14ac:dyDescent="0.3">
+      <c r="E27" s="7">
+        <v>76.739000000000004</v>
+      </c>
+      <c r="F27" s="11">
+        <v>0.9813171355498721</v>
+      </c>
+      <c r="G27" s="12">
+        <v>0.15079644737231007</v>
+      </c>
+      <c r="H27" s="11">
+        <v>7.595477208004076</v>
+      </c>
+    </row>
+    <row r="28" spans="5:8" x14ac:dyDescent="0.3">
+      <c r="E28" s="7">
+        <v>163.584</v>
+      </c>
+      <c r="F28" s="11">
+        <v>1.0138456770994733</v>
+      </c>
+      <c r="G28" s="12">
+        <v>0.18535396656179778</v>
+      </c>
+      <c r="H28" s="11">
+        <v>6.1381358879249017</v>
       </c>
     </row>
   </sheetData>

</xml_diff>